<commit_message>
spreadsheets:add csv support and more tests
</commit_message>
<xml_diff>
--- a/modules/spreadsheets/src/test/resources/sample.xlsx
+++ b/modules/spreadsheets/src/test/resources/sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>a</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>partner</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>expected</t>
   </si>
 </sst>
 </file>
@@ -370,7 +376,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C1" sqref="C1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -415,12 +421,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42.01</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>